<commit_message>
Update partnership alignment process
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\regression models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC140C83-7903-479D-892F-675133D66666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0054E0C-F6CA-4578-828A-8D5B5E651F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
     <sheet name="social care" sheetId="1" r:id="rId2"/>
-    <sheet name="raw data" sheetId="3" r:id="rId3"/>
+    <sheet name="partnership" sheetId="4" r:id="rId3"/>
+    <sheet name="raw data" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>CAPITAL LIMITS</t>
   </si>
@@ -143,6 +144,9 @@
   </si>
   <si>
     <t>MINIMUM INCOME GUARANTEE PER WEEK</t>
+  </si>
+  <si>
+    <t>partnered_share</t>
   </si>
 </sst>
 </file>
@@ -579,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5A30919-82CE-4DA6-A5C0-32D0B4E57BD6}">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1012,6 +1016,173 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.62972779999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.62818549999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.62484090000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.61718680000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.61729670000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.61867839999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.60632839999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.60035260000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.58782400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.58603729999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA85A294-76F0-4023-B97D-1E7832E0E774}">
   <dimension ref="A1:U16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Draft version of activity alignment procedure
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0054E0C-F6CA-4578-828A-8D5B5E651F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D513C5F2-8088-4855-A64C-45E12E599E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
     <sheet name="social care" sheetId="1" r:id="rId2"/>
     <sheet name="partnership" sheetId="4" r:id="rId3"/>
-    <sheet name="raw data" sheetId="3" r:id="rId4"/>
+    <sheet name="employment" sheetId="5" r:id="rId4"/>
+    <sheet name="raw data" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>CAPITAL LIMITS</t>
   </si>
@@ -147,6 +148,9 @@
   </si>
   <si>
     <t>partnered_share</t>
+  </si>
+  <si>
+    <t>employed_share</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1183,6 +1187,173 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02B2D7-F4EC-4D40-840B-FB6BA99B9F2B}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA85A294-76F0-4023-B97D-1E7832E0E774}">
   <dimension ref="A1:U16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Working activity status alignment
-Still needs targets to be updated from the data
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D513C5F2-8088-4855-A64C-45E12E599E91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB796045-FB96-4382-B2DA-02E847EFBDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
     <sheet name="social care" sheetId="1" r:id="rId2"/>
     <sheet name="partnership" sheetId="4" r:id="rId3"/>
-    <sheet name="employment" sheetId="5" r:id="rId4"/>
-    <sheet name="raw data" sheetId="3" r:id="rId5"/>
+    <sheet name="employment_smales" sheetId="5" r:id="rId4"/>
+    <sheet name="employment_sfemales" sheetId="6" r:id="rId5"/>
+    <sheet name="employment_couples" sheetId="7" r:id="rId6"/>
+    <sheet name="raw data" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>CAPITAL LIMITS</t>
   </si>
@@ -1190,6 +1192,173 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C02B2D7-F4EC-4D40-840B-FB6BA99B9F2B}">
   <dimension ref="A1:B19"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -1209,7 +1378,7 @@
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1217,7 +1386,7 @@
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1225,7 +1394,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1233,7 +1402,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1241,7 +1410,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1249,7 +1418,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1257,7 +1426,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1265,7 +1434,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1273,7 +1442,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1281,7 +1450,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1289,7 +1458,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1297,7 +1466,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1305,7 +1474,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1313,7 +1482,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1321,7 +1490,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1329,7 +1498,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1337,7 +1506,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1345,7 +1514,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -1353,7 +1522,174 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA85A294-76F0-4023-B97D-1E7832E0E774}">
   <dimension ref="A1:U16"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update activity alignment process
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB796045-FB96-4382-B2DA-02E847EFBDBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4885F50-CDFF-49FF-99FA-7227C7C22906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="12750" yWindow="1710" windowWidth="21900" windowHeight="15510" firstSheet="2" activeTab="5" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -1193,6 +1193,173 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0.53940549999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0.54004809999999992</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0.55193539999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0.57619909999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0.57942509999999992</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0.57820819999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1211,7 +1378,7 @@
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>0.6</v>
+        <v>0.39165939999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1219,7 +1386,7 @@
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>0.6</v>
+        <v>0.40846290000000002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1227,7 +1394,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.41123969999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1235,7 +1402,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0.6</v>
+        <v>0.43660460000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1243,7 +1410,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0.6</v>
+        <v>0.44596649999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1251,7 +1418,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1259,7 +1426,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1267,7 +1434,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1275,7 +1442,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1283,7 +1450,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1291,7 +1458,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1299,7 +1466,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1307,7 +1474,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1315,7 +1482,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1323,7 +1490,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1331,7 +1498,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1339,7 +1506,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1347,7 +1514,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0.6</v>
+        <v>0.45383590000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1355,8 +1522,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ADCB18-5B9A-4019-89E5-BA38EA9BE54A}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1378,7 +1545,7 @@
         <v>2010</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.71755429999999998</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1386,7 +1553,7 @@
         <v>2011</v>
       </c>
       <c r="B3">
-        <v>0.4</v>
+        <v>0.73036599999999996</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1394,7 +1561,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0.4</v>
+        <v>0.74233179999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1402,7 +1569,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0.4</v>
+        <v>0.74778829999999996</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1410,7 +1577,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0.4</v>
+        <v>0.74564959999999991</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1418,7 +1585,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0.4</v>
+        <v>0.74624679999999999</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1426,7 +1593,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1434,7 +1601,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1442,7 +1609,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1450,7 +1617,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1458,7 +1625,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1466,7 +1633,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1474,7 +1641,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1482,7 +1649,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1490,7 +1657,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1498,7 +1665,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1506,7 +1673,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0.4</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1514,174 +1681,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0.4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
-  <dimension ref="A1:B19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
-      </c>
-      <c r="B3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="B4">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="B5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="B7">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2018</v>
-      </c>
-      <c r="B10">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2019</v>
-      </c>
-      <c r="B11">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
-      </c>
-      <c r="B13">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2022</v>
-      </c>
-      <c r="B14">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>2023</v>
-      </c>
-      <c r="B15">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2024</v>
-      </c>
-      <c r="B16">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2025</v>
-      </c>
-      <c r="B17">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2026</v>
-      </c>
-      <c r="B18">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2027</v>
-      </c>
-      <c r="B19">
-        <v>0.6</v>
+        <v>0.74345260000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update population and cohabitation targets
</commit_message>
<xml_diff>
--- a/input/policy parameters.xlsx
+++ b/input/policy parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4885F50-CDFF-49FF-99FA-7227C7C22906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C55D118-45C5-4278-B5B4-5D567E3F435B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12750" yWindow="1710" windowWidth="21900" windowHeight="15510" firstSheet="2" activeTab="5" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E29F3EB7-07F0-4B2F-ABCD-03E4363B7DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
   <si>
     <t>CAPITAL LIMITS</t>
   </si>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t>employed_share</t>
+  </si>
+  <si>
+    <t>26/08/2024 (JV)</t>
+  </si>
+  <si>
+    <t>partnership:</t>
+  </si>
+  <si>
+    <t>rates evaluated from proportions benefit units of weight FRS population described as "couple" (registered married + civil partnershp + cohabiting couples) (variable famtypbu) - see raw data tab</t>
+  </si>
+  <si>
+    <t>proportion FRS Benefit Units cohabiting</t>
+  </si>
+  <si>
+    <t>Implied proportion of responsible adults in cohabiting relationship</t>
   </si>
 </sst>
 </file>
@@ -197,10 +212,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -219,9 +235,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -259,7 +275,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -365,7 +381,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -507,7 +523,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F81ED4-EE1A-4486-BAEC-BC92A19478AC}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,7 +572,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -578,6 +594,14 @@
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1023,11 +1047,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8252C88-1FFA-4D3B-9F14-2D9286827575}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1040,147 +1062,243 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
+        <v>1994</v>
+      </c>
+      <c r="B2">
+        <v>0.6613654059472992</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1995</v>
+      </c>
+      <c r="B3">
+        <v>0.65666662435166534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1996</v>
+      </c>
+      <c r="B4">
+        <v>0.65162882226991414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1997</v>
+      </c>
+      <c r="B5">
+        <v>0.64942413470967808</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1998</v>
+      </c>
+      <c r="B6">
+        <v>0.64547705146902756</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1999</v>
+      </c>
+      <c r="B7">
+        <v>0.64460168570888343</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B8">
+        <v>0.64477324955863657</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>2001</v>
+      </c>
+      <c r="B9">
+        <v>0.64570195231543648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>2002</v>
+      </c>
+      <c r="B10">
+        <v>0.64737782355652385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>2003</v>
+      </c>
+      <c r="B11">
+        <v>0.64448143654604106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>2004</v>
+      </c>
+      <c r="B12">
+        <v>0.64389807700679014</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>2005</v>
+      </c>
+      <c r="B13">
+        <v>0.63601678163112885</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>2006</v>
+      </c>
+      <c r="B14">
+        <v>0.63885715724636716</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>2007</v>
+      </c>
+      <c r="B15">
+        <v>0.63970331929393809</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>2008</v>
+      </c>
+      <c r="B16">
+        <v>0.63745385907812036</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>2009</v>
+      </c>
+      <c r="B17">
+        <v>0.64638142900294271</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>2010</v>
       </c>
-      <c r="B2">
-        <v>0.62972779999999995</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="B18">
+        <v>0.64291910814000863</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>2011</v>
       </c>
-      <c r="B3">
-        <v>0.62818549999999995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="B19">
+        <v>0.64183543445918845</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>2012</v>
       </c>
-      <c r="B4">
-        <v>0.62484090000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="B20">
+        <v>0.64457311813040019</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>2013</v>
       </c>
-      <c r="B5">
-        <v>0.61718680000000004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="B21">
+        <v>0.64501821298769013</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>2014</v>
       </c>
-      <c r="B6">
-        <v>0.61729670000000003</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B22">
+        <v>0.64303300577959377</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>2015</v>
       </c>
-      <c r="B7">
-        <v>0.61867839999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B23">
+        <v>0.64350137796521267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>2016</v>
       </c>
-      <c r="B8">
-        <v>0.60632839999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B24">
+        <v>0.64443090532156433</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>2017</v>
       </c>
-      <c r="B9">
-        <v>0.60035260000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="B25">
+        <v>0.64369538754708922</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>2018</v>
       </c>
-      <c r="B10">
-        <v>0.58782400000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="B26">
+        <v>0.64389678969687036</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>2019</v>
       </c>
-      <c r="B11">
-        <v>0.58603729999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="B27">
+        <v>0.63975244582712099</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>2020</v>
       </c>
-      <c r="B12">
-        <v>0.58603729999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="B28">
+        <v>0.64948824720523413</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>2021</v>
       </c>
-      <c r="B13">
-        <v>0.58603729999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="B29">
+        <v>0.64443733677754689</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>2022</v>
       </c>
-      <c r="B14">
-        <v>0.58603729999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="B30">
+        <v>0.64425404141077236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
         <v>2023</v>
       </c>
-      <c r="B15">
-        <v>0.58603729999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>2024</v>
-      </c>
-      <c r="B16">
-        <v>0.58603729999999998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>2025</v>
-      </c>
-      <c r="B17">
-        <v>0.58603729999999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>2026</v>
-      </c>
-      <c r="B18">
-        <v>0.58603729999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2027</v>
-      </c>
-      <c r="B19">
-        <v>0.58603729999999998</v>
+      <c r="B31">
+        <v>0.64425404141077236</v>
       </c>
     </row>
   </sheetData>
@@ -1526,7 +1644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D244153-91CD-4DE3-A3BE-886BB7506357}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1691,15 +1809,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA85A294-76F0-4023-B97D-1E7832E0E774}">
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="Y4" sqref="Y4:Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="23" max="26" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>34</v>
       </c>
@@ -1710,7 +1831,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -1726,7 +1847,7 @@
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1775,8 +1896,14 @@
       <c r="U3" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="X3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2015</v>
       </c>
@@ -1843,8 +1970,18 @@
         <f t="shared" si="0"/>
         <v>23250</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W4" s="3">
+        <v>1994</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0.49405969999999999</v>
+      </c>
+      <c r="Y4" s="3">
+        <f>2*X4/(2*X4+(1-X4))</f>
+        <v>0.6613654059472992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2016</v>
       </c>
@@ -1911,8 +2048,19 @@
         <f t="shared" ref="U5:U12" si="9">I5*$K$4/$K5</f>
         <v>23088.381330685203</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W5" s="3">
+        <f>W4+1</f>
+        <v>1995</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0.48883369999999998</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" ref="Y5:Y31" si="10">2*X5/(2*X5+(1-X5))</f>
+        <v>0.65666662435166534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2017</v>
       </c>
@@ -1979,8 +2127,19 @@
         <f t="shared" si="9"/>
         <v>22485.493230174081</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W6" s="3">
+        <f t="shared" ref="W6:W42" si="11">W5+1</f>
+        <v>1996</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0.48327110000000001</v>
+      </c>
+      <c r="Y6" s="3">
+        <f t="shared" si="10"/>
+        <v>0.65162882226991414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2018</v>
       </c>
@@ -2047,8 +2206,19 @@
         <f t="shared" si="9"/>
         <v>21954.67422096317</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W7" s="3">
+        <f t="shared" si="11"/>
+        <v>1997</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0.48084979999999999</v>
+      </c>
+      <c r="Y7" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64942413470967808</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2019</v>
       </c>
@@ -2115,8 +2285,19 @@
         <f t="shared" si="9"/>
         <v>21567.717996289426</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W8" s="3">
+        <f t="shared" si="11"/>
+        <v>1998</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0.47653459999999997</v>
+      </c>
+      <c r="Y8" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64547705146902756</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2020</v>
       </c>
@@ -2183,8 +2364,19 @@
         <f t="shared" si="9"/>
         <v>21389.144434222631</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W9" s="3">
+        <f t="shared" si="11"/>
+        <v>1999</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0.47558099999999998</v>
+      </c>
+      <c r="Y9" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64460168570888343</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -2251,8 +2443,19 @@
         <f t="shared" si="9"/>
         <v>20833.333333333336</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W10" s="3">
+        <f t="shared" si="11"/>
+        <v>2000</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0.47576780000000002</v>
+      </c>
+      <c r="Y10" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64477324955863657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -2319,8 +2522,19 @@
         <f t="shared" si="9"/>
         <v>19104.354971240755</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W11" s="3">
+        <f t="shared" si="11"/>
+        <v>2001</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0.47677979999999998</v>
+      </c>
+      <c r="Y11" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64570195231543648</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2023</v>
       </c>
@@ -2387,8 +2601,19 @@
         <f t="shared" si="9"/>
         <v>18663.611748853393</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="W12" s="3">
+        <f t="shared" si="11"/>
+        <v>2002</v>
+      </c>
+      <c r="X12" s="3">
+        <v>0.47860950000000002</v>
+      </c>
+      <c r="Y12" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64737782355652385</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2024</v>
       </c>
@@ -2410,35 +2635,46 @@
         <v>83.203585280372224</v>
       </c>
       <c r="O13" s="2">
-        <f t="shared" ref="O13:S13" si="10">O12</f>
+        <f t="shared" ref="O13:S13" si="12">O12</f>
         <v>172.06645928459034</v>
       </c>
       <c r="P13" s="2">
+        <f t="shared" si="12"/>
+        <v>36.725171505808291</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="12"/>
+        <v>65.342709520716838</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="12"/>
+        <v>131.36774463225194</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="12"/>
+        <v>26.169193247854651</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" ref="T13:T16" si="13">H13*$K$4/$K13</f>
+        <v>11253.200432308387</v>
+      </c>
+      <c r="U13" s="2">
+        <f t="shared" ref="U13:U16" si="14">I13*$K$4/$K13</f>
+        <v>18360.484915871581</v>
+      </c>
+      <c r="W13" s="3">
+        <f t="shared" si="11"/>
+        <v>2003</v>
+      </c>
+      <c r="X13" s="3">
+        <v>0.47545009999999999</v>
+      </c>
+      <c r="Y13" s="3">
         <f t="shared" si="10"/>
-        <v>36.725171505808291</v>
-      </c>
-      <c r="Q13" s="2">
-        <f t="shared" si="10"/>
-        <v>65.342709520716838</v>
-      </c>
-      <c r="R13" s="2">
-        <f t="shared" si="10"/>
-        <v>131.36774463225194</v>
-      </c>
-      <c r="S13" s="2">
-        <f t="shared" si="10"/>
-        <v>26.169193247854651</v>
-      </c>
-      <c r="T13" s="2">
-        <f t="shared" ref="T13:T16" si="11">H13*$K$4/$K13</f>
-        <v>11253.200432308387</v>
-      </c>
-      <c r="U13" s="2">
-        <f t="shared" ref="U13:U16" si="12">I13*$K$4/$K13</f>
-        <v>18360.484915871581</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.64448143654604106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2025</v>
       </c>
@@ -2456,39 +2692,50 @@
         <v>2025</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" ref="N14:N16" si="13">N13</f>
+        <f t="shared" ref="N14:N16" si="15">N13</f>
         <v>83.203585280372224</v>
       </c>
       <c r="O14" s="2">
-        <f t="shared" ref="O14:O16" si="14">O13</f>
+        <f t="shared" ref="O14:O16" si="16">O13</f>
         <v>172.06645928459034</v>
       </c>
       <c r="P14" s="2">
-        <f t="shared" ref="P14:P16" si="15">P13</f>
+        <f t="shared" ref="P14:P16" si="17">P13</f>
         <v>36.725171505808291</v>
       </c>
       <c r="Q14" s="2">
-        <f t="shared" ref="Q14:Q16" si="16">Q13</f>
+        <f t="shared" ref="Q14:Q16" si="18">Q13</f>
         <v>65.342709520716838</v>
       </c>
       <c r="R14" s="2">
-        <f t="shared" ref="R14:R16" si="17">R13</f>
+        <f t="shared" ref="R14:R16" si="19">R13</f>
         <v>131.36774463225194</v>
       </c>
       <c r="S14" s="2">
-        <f t="shared" ref="S14:S16" si="18">S13</f>
+        <f t="shared" ref="S14:S16" si="20">S13</f>
         <v>26.169193247854651</v>
       </c>
       <c r="T14" s="2">
+        <f t="shared" si="13"/>
+        <v>11036.497686088615</v>
+      </c>
+      <c r="U14" s="2">
+        <f t="shared" si="14"/>
+        <v>18006.917277302477</v>
+      </c>
+      <c r="W14" s="3">
         <f t="shared" si="11"/>
-        <v>11036.497686088615</v>
-      </c>
-      <c r="U14" s="2">
-        <f t="shared" si="12"/>
-        <v>18006.917277302477</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2004</v>
+      </c>
+      <c r="X14" s="3">
+        <v>0.4748154</v>
+      </c>
+      <c r="Y14" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64389807700679014</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2026</v>
       </c>
@@ -2506,39 +2753,50 @@
         <v>2026</v>
       </c>
       <c r="N15" s="2">
+        <f t="shared" si="15"/>
+        <v>83.203585280372224</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="16"/>
+        <v>172.06645928459034</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="17"/>
+        <v>36.725171505808291</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="18"/>
+        <v>65.342709520716838</v>
+      </c>
+      <c r="R15" s="2">
+        <f t="shared" si="19"/>
+        <v>131.36774463225194</v>
+      </c>
+      <c r="S15" s="2">
+        <f t="shared" si="20"/>
+        <v>26.169193247854651</v>
+      </c>
+      <c r="T15" s="2">
         <f t="shared" si="13"/>
-        <v>83.203585280372224</v>
-      </c>
-      <c r="O15" s="2">
+        <v>10820.095770675114</v>
+      </c>
+      <c r="U15" s="2">
         <f t="shared" si="14"/>
-        <v>172.06645928459034</v>
-      </c>
-      <c r="P15" s="2">
-        <f t="shared" si="15"/>
-        <v>36.725171505808291</v>
-      </c>
-      <c r="Q15" s="2">
-        <f t="shared" si="16"/>
-        <v>65.342709520716838</v>
-      </c>
-      <c r="R15" s="2">
-        <f t="shared" si="17"/>
-        <v>131.36774463225194</v>
-      </c>
-      <c r="S15" s="2">
-        <f t="shared" si="18"/>
-        <v>26.169193247854651</v>
-      </c>
-      <c r="T15" s="2">
+        <v>17653.840467943606</v>
+      </c>
+      <c r="W15" s="3">
         <f t="shared" si="11"/>
-        <v>10820.095770675114</v>
-      </c>
-      <c r="U15" s="2">
-        <f t="shared" si="12"/>
-        <v>17653.840467943606</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>2005</v>
+      </c>
+      <c r="X15" s="3">
+        <v>0.46629369999999998</v>
+      </c>
+      <c r="Y15" s="3">
+        <f t="shared" si="10"/>
+        <v>0.63601678163112885</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2027</v>
       </c>
@@ -2556,36 +2814,260 @@
         <v>2027</v>
       </c>
       <c r="N16" s="2">
+        <f t="shared" si="15"/>
+        <v>83.203585280372224</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="16"/>
+        <v>172.06645928459034</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="17"/>
+        <v>36.725171505808291</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="18"/>
+        <v>65.342709520716838</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" si="19"/>
+        <v>131.36774463225194</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="20"/>
+        <v>26.169193247854651</v>
+      </c>
+      <c r="T16" s="2">
         <f t="shared" si="13"/>
-        <v>83.203585280372224</v>
-      </c>
-      <c r="O16" s="2">
+        <v>10545.581287705945</v>
+      </c>
+      <c r="U16" s="2">
         <f t="shared" si="14"/>
-        <v>172.06645928459034</v>
-      </c>
-      <c r="P16" s="2">
-        <f t="shared" si="15"/>
-        <v>36.725171505808291</v>
-      </c>
-      <c r="Q16" s="2">
-        <f t="shared" si="16"/>
-        <v>65.342709520716838</v>
-      </c>
-      <c r="R16" s="2">
-        <f t="shared" si="17"/>
-        <v>131.36774463225194</v>
-      </c>
-      <c r="S16" s="2">
-        <f t="shared" si="18"/>
-        <v>26.169193247854651</v>
-      </c>
-      <c r="T16" s="2">
+        <v>17205.948416783383</v>
+      </c>
+      <c r="W16" s="3">
         <f t="shared" si="11"/>
-        <v>10545.581287705945</v>
-      </c>
-      <c r="U16" s="2">
-        <f t="shared" si="12"/>
-        <v>17205.948416783383</v>
+        <v>2006</v>
+      </c>
+      <c r="X16" s="3">
+        <v>0.46935349999999998</v>
+      </c>
+      <c r="Y16" s="3">
+        <f t="shared" si="10"/>
+        <v>0.63885715724636716</v>
+      </c>
+    </row>
+    <row r="17" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W17" s="3">
+        <f t="shared" si="11"/>
+        <v>2007</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0.4702675</v>
+      </c>
+      <c r="Y17" s="3">
+        <f t="shared" si="10"/>
+        <v>0.63970331929393809</v>
+      </c>
+    </row>
+    <row r="18" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W18" s="3">
+        <f t="shared" si="11"/>
+        <v>2008</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0.46784019999999998</v>
+      </c>
+      <c r="Y18" s="3">
+        <f t="shared" si="10"/>
+        <v>0.63745385907812036</v>
+      </c>
+    </row>
+    <row r="19" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W19" s="3">
+        <f t="shared" si="11"/>
+        <v>2009</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0.47752109999999998</v>
+      </c>
+      <c r="Y19" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64638142900294271</v>
+      </c>
+    </row>
+    <row r="20" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W20" s="3">
+        <f t="shared" si="11"/>
+        <v>2010</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0.47375149999999999</v>
+      </c>
+      <c r="Y20" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64291910814000863</v>
+      </c>
+    </row>
+    <row r="21" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W21" s="3">
+        <f t="shared" si="11"/>
+        <v>2011</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0.47257559999999998</v>
+      </c>
+      <c r="Y21" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64183543445918845</v>
+      </c>
+    </row>
+    <row r="22" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W22" s="3">
+        <f t="shared" si="11"/>
+        <v>2012</v>
+      </c>
+      <c r="X22" s="3">
+        <v>0.47554990000000003</v>
+      </c>
+      <c r="Y22" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64457311813040019</v>
+      </c>
+    </row>
+    <row r="23" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W23" s="3">
+        <f t="shared" si="11"/>
+        <v>2013</v>
+      </c>
+      <c r="X23" s="3">
+        <v>0.47603459999999997</v>
+      </c>
+      <c r="Y23" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64501821298769013</v>
+      </c>
+    </row>
+    <row r="24" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W24" s="3">
+        <f t="shared" si="11"/>
+        <v>2014</v>
+      </c>
+      <c r="X24" s="3">
+        <v>0.4738752</v>
+      </c>
+      <c r="Y24" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64303300577959377</v>
+      </c>
+    </row>
+    <row r="25" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W25" s="3">
+        <f t="shared" si="11"/>
+        <v>2015</v>
+      </c>
+      <c r="X25" s="3">
+        <v>0.47438409999999998</v>
+      </c>
+      <c r="Y25" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64350137796521267</v>
+      </c>
+    </row>
+    <row r="26" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W26" s="3">
+        <f t="shared" si="11"/>
+        <v>2016</v>
+      </c>
+      <c r="X26" s="3">
+        <v>0.47539510000000001</v>
+      </c>
+      <c r="Y26" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64443090532156433</v>
+      </c>
+    </row>
+    <row r="27" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W27" s="3">
+        <f t="shared" si="11"/>
+        <v>2017</v>
+      </c>
+      <c r="X27" s="3">
+        <v>0.47459499999999999</v>
+      </c>
+      <c r="Y27" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64369538754708922</v>
+      </c>
+    </row>
+    <row r="28" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W28" s="3">
+        <f t="shared" si="11"/>
+        <v>2018</v>
+      </c>
+      <c r="X28" s="3">
+        <v>0.47481400000000001</v>
+      </c>
+      <c r="Y28" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64389678969687036</v>
+      </c>
+    </row>
+    <row r="29" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W29" s="3">
+        <f t="shared" si="11"/>
+        <v>2019</v>
+      </c>
+      <c r="X29" s="3">
+        <v>0.47032059999999998</v>
+      </c>
+      <c r="Y29" s="3">
+        <f t="shared" si="10"/>
+        <v>0.63975244582712099</v>
+      </c>
+    </row>
+    <row r="30" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W30" s="3">
+        <f t="shared" si="11"/>
+        <v>2020</v>
+      </c>
+      <c r="X30" s="3">
+        <v>0.48092010000000002</v>
+      </c>
+      <c r="Y30" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64948824720523413</v>
+      </c>
+    </row>
+    <row r="31" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W31" s="3">
+        <f t="shared" si="11"/>
+        <v>2021</v>
+      </c>
+      <c r="X31" s="3">
+        <v>0.47540209999999999</v>
+      </c>
+      <c r="Y31" s="3">
+        <f t="shared" si="10"/>
+        <v>0.64443733677754689</v>
+      </c>
+    </row>
+    <row r="32" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W32" s="3">
+        <v>2022</v>
+      </c>
+      <c r="Y32" s="3">
+        <f>AVERAGE(Y27:Y31)</f>
+        <v>0.64425404141077236</v>
+      </c>
+    </row>
+    <row r="33" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W33" s="3">
+        <v>2023</v>
+      </c>
+      <c r="Y33" s="3">
+        <f>Y32</f>
+        <v>0.64425404141077236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>